<commit_message>
cookbook updates for reworked data model
</commit_message>
<xml_diff>
--- a/doc/user-guide/cookbook/calendar/calendar-working-hours.xlsx
+++ b/doc/user-guide/cookbook/calendar/calendar-working-hours.xlsx
@@ -5,33 +5,32 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\develop\frepple-community-4.0\doc\cookbook\calendar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\develop\frepple-community-4.0\doc\user-guide\cookbook\calendar\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="135" yWindow="563" windowWidth="22718" windowHeight="11055" tabRatio="729" activeTab="8"/>
   </bookViews>
   <sheets>
-    <sheet name="item operation" sheetId="13" r:id="rId1"/>
-    <sheet name="calendar bucket" sheetId="2" r:id="rId2"/>
-    <sheet name="calendar" sheetId="3" r:id="rId3"/>
-    <sheet name="demand" sheetId="4" r:id="rId4"/>
-    <sheet name="customer" sheetId="12" r:id="rId5"/>
-    <sheet name="operation material" sheetId="5" r:id="rId6"/>
-    <sheet name="item distribution" sheetId="14" r:id="rId7"/>
-    <sheet name="item" sheetId="6" r:id="rId8"/>
-    <sheet name="location" sheetId="7" r:id="rId9"/>
-    <sheet name="operation" sheetId="8" r:id="rId10"/>
-    <sheet name="bucket date" sheetId="9" r:id="rId11"/>
-    <sheet name="bucket" sheetId="10" r:id="rId12"/>
-    <sheet name="parameter" sheetId="11" r:id="rId13"/>
+    <sheet name="calendar bucket" sheetId="2" r:id="rId1"/>
+    <sheet name="calendar" sheetId="3" r:id="rId2"/>
+    <sheet name="demand" sheetId="4" r:id="rId3"/>
+    <sheet name="customer" sheetId="12" r:id="rId4"/>
+    <sheet name="operation material" sheetId="5" r:id="rId5"/>
+    <sheet name="item distribution" sheetId="14" r:id="rId6"/>
+    <sheet name="item" sheetId="6" r:id="rId7"/>
+    <sheet name="location" sheetId="7" r:id="rId8"/>
+    <sheet name="operation" sheetId="8" r:id="rId9"/>
+    <sheet name="bucket date" sheetId="9" r:id="rId10"/>
+    <sheet name="bucket" sheetId="10" r:id="rId11"/>
+    <sheet name="parameter" sheetId="11" r:id="rId12"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14050" uniqueCount="6474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14046" uniqueCount="6474">
   <si>
     <t>name</t>
   </si>
@@ -19797,39 +19796,192 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>6470</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>6472</v>
+        <v>25</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2" t="b">
+        <v>0</v>
+      </c>
+      <c r="L2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>9</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L3" t="b">
+        <v>0</v>
+      </c>
+      <c r="M3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>8</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4" t="b">
+        <v>1</v>
+      </c>
+      <c r="L4" t="b">
+        <v>1</v>
+      </c>
+      <c r="M4" t="s">
+        <v>32</v>
+      </c>
+      <c r="N4" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -19838,79 +19990,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>6472</v>
-      </c>
-      <c r="B2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6470</v>
-      </c>
-      <c r="D2">
-        <v>172800</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3">
-        <v>172800</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3484"/>
   <sheetViews>
@@ -79153,7 +79232,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -79238,7 +79317,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -79281,201 +79360,6 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="12.796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="18.1328125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>10</v>
-      </c>
-      <c r="F2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J2" t="b">
-        <v>1</v>
-      </c>
-      <c r="K2" t="b">
-        <v>0</v>
-      </c>
-      <c r="L2" t="b">
-        <v>0</v>
-      </c>
-      <c r="M2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>9</v>
-      </c>
-      <c r="F3" t="b">
-        <v>1</v>
-      </c>
-      <c r="G3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J3" t="b">
-        <v>1</v>
-      </c>
-      <c r="K3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L3" t="b">
-        <v>0</v>
-      </c>
-      <c r="M3" t="s">
-        <v>28</v>
-      </c>
-      <c r="N3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>8</v>
-      </c>
-      <c r="F4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H4" t="b">
-        <v>1</v>
-      </c>
-      <c r="I4" t="b">
-        <v>1</v>
-      </c>
-      <c r="J4" t="b">
-        <v>1</v>
-      </c>
-      <c r="K4" t="b">
-        <v>1</v>
-      </c>
-      <c r="L4" t="b">
-        <v>1</v>
-      </c>
-      <c r="M4" t="s">
-        <v>32</v>
-      </c>
-      <c r="N4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -79516,7 +79400,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
@@ -79583,7 +79467,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -79608,7 +79492,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -79669,7 +79553,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -79706,7 +79590,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -79737,11 +79621,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -79777,4 +79661,84 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>6472</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6470</v>
+      </c>
+      <c r="E2">
+        <v>172800</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <v>172800</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>